<commit_message>
Additional electricity profile shit
</commit_message>
<xml_diff>
--- a/Electricity.xlsx
+++ b/Electricity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9CE1BF-86F6-4818-866C-2A25288D204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF0E5D-3231-49E9-9C65-CA14C400ECDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -538,30 +538,6 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,21 +586,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,6 +608,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AB632A-CF7E-4474-8575-35E9A95F1781}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1435,2084 +1435,2084 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EEF8B1-E0DF-4071-B506-FDD79B5129C3}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="7.90625" style="29" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="7.26953125" style="29" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.7265625" style="29"/>
+    <col min="1" max="1" width="15.7265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="7.90625" style="21" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="7.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.7265625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="26" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="26" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="26" t="s">
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="26" t="s">
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="26" t="s">
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="26" t="s">
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="28"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="47"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="49"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="31" t="s">
+      <c r="R2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="31" t="s">
+      <c r="S2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="32" t="s">
+      <c r="U2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="31" t="s">
+      <c r="X2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="Y2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="32" t="s">
+      <c r="Z2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="AB2" s="31" t="s">
+      <c r="AB2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AC2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="31" t="s">
+      <c r="AD2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" s="32" t="s">
+      <c r="AE2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AF2" s="30" t="s">
+      <c r="AF2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="AG2" s="31" t="s">
+      <c r="AG2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="31" t="s">
+      <c r="AH2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AI2" s="31" t="s">
+      <c r="AI2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="32" t="s">
+      <c r="AJ2" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="55">
-        <v>0</v>
-      </c>
-      <c r="C3" s="56">
+      <c r="B3" s="42">
+        <v>0</v>
+      </c>
+      <c r="C3" s="43">
         <v>0.25</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="43">
         <v>0.5</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="44">
         <v>0.91666666666666663</v>
       </c>
-      <c r="G3" s="55">
-        <v>0</v>
-      </c>
-      <c r="H3" s="56">
+      <c r="G3" s="42">
+        <v>0</v>
+      </c>
+      <c r="H3" s="43">
         <v>0.25</v>
       </c>
-      <c r="I3" s="56">
+      <c r="I3" s="43">
         <v>0.5</v>
       </c>
-      <c r="J3" s="56">
+      <c r="J3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K3" s="57">
+      <c r="K3" s="44">
         <v>0.91666666666666663</v>
       </c>
-      <c r="L3" s="55">
-        <v>0</v>
-      </c>
-      <c r="M3" s="56">
+      <c r="L3" s="42">
+        <v>0</v>
+      </c>
+      <c r="M3" s="43">
         <v>0.25</v>
       </c>
-      <c r="N3" s="56">
+      <c r="N3" s="43">
         <v>0.5</v>
       </c>
-      <c r="O3" s="56">
+      <c r="O3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="P3" s="57">
+      <c r="P3" s="44">
         <v>0.91666666666666663</v>
       </c>
-      <c r="Q3" s="55">
-        <v>0</v>
-      </c>
-      <c r="R3" s="56">
+      <c r="Q3" s="42">
+        <v>0</v>
+      </c>
+      <c r="R3" s="43">
         <v>0.25</v>
       </c>
-      <c r="S3" s="56">
+      <c r="S3" s="43">
         <v>0.5</v>
       </c>
-      <c r="T3" s="56">
+      <c r="T3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="U3" s="57">
+      <c r="U3" s="44">
         <v>0.91666666666666663</v>
       </c>
-      <c r="V3" s="55">
-        <v>0</v>
-      </c>
-      <c r="W3" s="56">
+      <c r="V3" s="42">
+        <v>0</v>
+      </c>
+      <c r="W3" s="43">
         <v>0.25</v>
       </c>
-      <c r="X3" s="56">
+      <c r="X3" s="43">
         <v>0.5</v>
       </c>
-      <c r="Y3" s="56">
+      <c r="Y3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="Z3" s="57">
+      <c r="Z3" s="44">
         <v>0.91666666666666663</v>
       </c>
-      <c r="AA3" s="55">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="56">
+      <c r="AA3" s="42">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="43">
         <v>0.25</v>
       </c>
-      <c r="AC3" s="56">
+      <c r="AC3" s="43">
         <v>0.5</v>
       </c>
-      <c r="AD3" s="56">
+      <c r="AD3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="AE3" s="57">
+      <c r="AE3" s="44">
         <v>0.91666666666666663</v>
       </c>
-      <c r="AF3" s="55">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="56">
+      <c r="AF3" s="42">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="43">
         <v>0.25</v>
       </c>
-      <c r="AH3" s="56">
+      <c r="AH3" s="43">
         <v>0.5</v>
       </c>
-      <c r="AI3" s="56">
+      <c r="AI3" s="43">
         <v>0.70833333333333337</v>
       </c>
-      <c r="AJ3" s="57">
+      <c r="AJ3" s="44">
         <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="51">
-        <v>0</v>
-      </c>
-      <c r="C4" s="52">
-        <v>1</v>
-      </c>
-      <c r="D4" s="52">
-        <v>0</v>
-      </c>
-      <c r="E4" s="52">
-        <v>1</v>
-      </c>
-      <c r="F4" s="53">
-        <v>0</v>
-      </c>
-      <c r="G4" s="51">
-        <v>0</v>
-      </c>
-      <c r="H4" s="52">
-        <v>1</v>
-      </c>
-      <c r="I4" s="52">
-        <v>0</v>
-      </c>
-      <c r="J4" s="52">
-        <v>1</v>
-      </c>
-      <c r="K4" s="53">
-        <v>0</v>
-      </c>
-      <c r="L4" s="51">
-        <v>0</v>
-      </c>
-      <c r="M4" s="52">
-        <v>1</v>
-      </c>
-      <c r="N4" s="52">
-        <v>0</v>
-      </c>
-      <c r="O4" s="52">
-        <v>1</v>
-      </c>
-      <c r="P4" s="53">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="51">
-        <v>0</v>
-      </c>
-      <c r="R4" s="52">
-        <v>1</v>
-      </c>
-      <c r="S4" s="52">
-        <v>0</v>
-      </c>
-      <c r="T4" s="52">
-        <v>1</v>
-      </c>
-      <c r="U4" s="53">
-        <v>0</v>
-      </c>
-      <c r="V4" s="51">
-        <v>0</v>
-      </c>
-      <c r="W4" s="52">
-        <v>1</v>
-      </c>
-      <c r="X4" s="52">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="52">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="53">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="51">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="52">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="52">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="52">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="53">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="51">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="52">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="52">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="52">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="53">
+      <c r="B4" s="38">
+        <v>1</v>
+      </c>
+      <c r="C4" s="39">
+        <v>1</v>
+      </c>
+      <c r="D4" s="39">
+        <v>0</v>
+      </c>
+      <c r="E4" s="39">
+        <v>1</v>
+      </c>
+      <c r="F4" s="40">
+        <v>0</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0</v>
+      </c>
+      <c r="H4" s="39">
+        <v>1</v>
+      </c>
+      <c r="I4" s="39">
+        <v>0</v>
+      </c>
+      <c r="J4" s="39">
+        <v>1</v>
+      </c>
+      <c r="K4" s="40">
+        <v>0</v>
+      </c>
+      <c r="L4" s="38">
+        <v>0</v>
+      </c>
+      <c r="M4" s="39">
+        <v>1</v>
+      </c>
+      <c r="N4" s="39">
+        <v>0</v>
+      </c>
+      <c r="O4" s="39">
+        <v>1</v>
+      </c>
+      <c r="P4" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="38">
+        <v>0</v>
+      </c>
+      <c r="R4" s="39">
+        <v>1</v>
+      </c>
+      <c r="S4" s="39">
+        <v>0</v>
+      </c>
+      <c r="T4" s="39">
+        <v>1</v>
+      </c>
+      <c r="U4" s="40">
+        <v>0</v>
+      </c>
+      <c r="V4" s="38">
+        <v>0</v>
+      </c>
+      <c r="W4" s="39">
+        <v>1</v>
+      </c>
+      <c r="X4" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="39">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="40">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="38">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="38">
-        <v>0</v>
-      </c>
-      <c r="C5" s="39">
-        <v>0</v>
-      </c>
-      <c r="D5" s="39">
-        <v>0</v>
-      </c>
-      <c r="E5" s="39">
-        <v>1</v>
-      </c>
-      <c r="F5" s="40">
-        <v>0</v>
-      </c>
-      <c r="G5" s="38">
-        <v>0</v>
-      </c>
-      <c r="H5" s="39">
-        <v>0</v>
-      </c>
-      <c r="I5" s="39">
-        <v>0</v>
-      </c>
-      <c r="J5" s="39">
-        <v>1</v>
-      </c>
-      <c r="K5" s="40">
-        <v>0</v>
-      </c>
-      <c r="L5" s="38">
-        <v>0</v>
-      </c>
-      <c r="M5" s="39">
-        <v>0</v>
-      </c>
-      <c r="N5" s="39">
-        <v>0</v>
-      </c>
-      <c r="O5" s="39">
-        <v>1</v>
-      </c>
-      <c r="P5" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="38">
-        <v>0</v>
-      </c>
-      <c r="R5" s="39">
-        <v>0</v>
-      </c>
-      <c r="S5" s="39">
-        <v>0</v>
-      </c>
-      <c r="T5" s="39">
-        <v>1</v>
-      </c>
-      <c r="U5" s="40">
-        <v>0</v>
-      </c>
-      <c r="V5" s="38">
-        <v>0</v>
-      </c>
-      <c r="W5" s="39">
-        <v>0</v>
-      </c>
-      <c r="X5" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="39">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="39">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="39">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="40">
+      <c r="B5" s="30">
+        <v>0</v>
+      </c>
+      <c r="C5" s="31">
+        <v>0</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0</v>
+      </c>
+      <c r="E5" s="31">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0</v>
+      </c>
+      <c r="J5" s="31">
+        <v>1</v>
+      </c>
+      <c r="K5" s="32">
+        <v>0</v>
+      </c>
+      <c r="L5" s="30">
+        <v>0</v>
+      </c>
+      <c r="M5" s="31">
+        <v>0</v>
+      </c>
+      <c r="N5" s="31">
+        <v>0</v>
+      </c>
+      <c r="O5" s="31">
+        <v>1</v>
+      </c>
+      <c r="P5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="30">
+        <v>0</v>
+      </c>
+      <c r="R5" s="31">
+        <v>0</v>
+      </c>
+      <c r="S5" s="31">
+        <v>0</v>
+      </c>
+      <c r="T5" s="31">
+        <v>1</v>
+      </c>
+      <c r="U5" s="32">
+        <v>0</v>
+      </c>
+      <c r="V5" s="30">
+        <v>0</v>
+      </c>
+      <c r="W5" s="31">
+        <v>0</v>
+      </c>
+      <c r="X5" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="31">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="34">
-        <v>0</v>
-      </c>
-      <c r="C6" s="35">
-        <v>0</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0</v>
-      </c>
-      <c r="F6" s="36">
-        <v>0</v>
-      </c>
-      <c r="G6" s="34">
-        <v>0</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0</v>
-      </c>
-      <c r="J6" s="35">
-        <v>0</v>
-      </c>
-      <c r="K6" s="36">
-        <v>0</v>
-      </c>
-      <c r="L6" s="34">
-        <v>0</v>
-      </c>
-      <c r="M6" s="35">
-        <v>1</v>
-      </c>
-      <c r="N6" s="35">
-        <v>0</v>
-      </c>
-      <c r="O6" s="35">
-        <v>0</v>
-      </c>
-      <c r="P6" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="34">
-        <v>0</v>
-      </c>
-      <c r="R6" s="35">
-        <v>0</v>
-      </c>
-      <c r="S6" s="35">
-        <v>0</v>
-      </c>
-      <c r="T6" s="35">
-        <v>0</v>
-      </c>
-      <c r="U6" s="36">
-        <v>0</v>
-      </c>
-      <c r="V6" s="34">
-        <v>0</v>
-      </c>
-      <c r="W6" s="35">
-        <v>1</v>
-      </c>
-      <c r="X6" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="36">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="35">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="36">
+      <c r="B6" s="26">
+        <v>0</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0</v>
+      </c>
+      <c r="J6" s="27">
+        <v>0</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0</v>
+      </c>
+      <c r="L6" s="26">
+        <v>0</v>
+      </c>
+      <c r="M6" s="27">
+        <v>1</v>
+      </c>
+      <c r="N6" s="27">
+        <v>0</v>
+      </c>
+      <c r="O6" s="27">
+        <v>0</v>
+      </c>
+      <c r="P6" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>0</v>
+      </c>
+      <c r="R6" s="27">
+        <v>0</v>
+      </c>
+      <c r="S6" s="27">
+        <v>0</v>
+      </c>
+      <c r="T6" s="27">
+        <v>0</v>
+      </c>
+      <c r="U6" s="28">
+        <v>0</v>
+      </c>
+      <c r="V6" s="26">
+        <v>0</v>
+      </c>
+      <c r="W6" s="27">
+        <v>1</v>
+      </c>
+      <c r="X6" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="28">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="28">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="38">
-        <v>0</v>
-      </c>
-      <c r="C7" s="39">
-        <v>0</v>
-      </c>
-      <c r="D7" s="39">
-        <v>0</v>
-      </c>
-      <c r="E7" s="39">
-        <v>0</v>
-      </c>
-      <c r="F7" s="40">
-        <v>0</v>
-      </c>
-      <c r="G7" s="38">
-        <v>0</v>
-      </c>
-      <c r="H7" s="39">
-        <v>0</v>
-      </c>
-      <c r="I7" s="39">
-        <v>0</v>
-      </c>
-      <c r="J7" s="39">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="38">
-        <v>0</v>
-      </c>
-      <c r="M7" s="39">
-        <v>0</v>
-      </c>
-      <c r="N7" s="39">
-        <v>0</v>
-      </c>
-      <c r="O7" s="39">
-        <v>0</v>
-      </c>
-      <c r="P7" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="38">
-        <v>0</v>
-      </c>
-      <c r="R7" s="39">
-        <v>0</v>
-      </c>
-      <c r="S7" s="39">
-        <v>0</v>
-      </c>
-      <c r="T7" s="39">
-        <v>0</v>
-      </c>
-      <c r="U7" s="40">
-        <v>0</v>
-      </c>
-      <c r="V7" s="38">
-        <v>0</v>
-      </c>
-      <c r="W7" s="39">
-        <v>0</v>
-      </c>
-      <c r="X7" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="40">
+      <c r="B7" s="30">
+        <v>0</v>
+      </c>
+      <c r="C7" s="31">
+        <v>0</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0</v>
+      </c>
+      <c r="J7" s="31">
+        <v>0</v>
+      </c>
+      <c r="K7" s="32">
+        <v>0</v>
+      </c>
+      <c r="L7" s="30">
+        <v>0</v>
+      </c>
+      <c r="M7" s="31">
+        <v>0</v>
+      </c>
+      <c r="N7" s="31">
+        <v>0</v>
+      </c>
+      <c r="O7" s="31">
+        <v>0</v>
+      </c>
+      <c r="P7" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>0</v>
+      </c>
+      <c r="R7" s="31">
+        <v>0</v>
+      </c>
+      <c r="S7" s="31">
+        <v>0</v>
+      </c>
+      <c r="T7" s="31">
+        <v>0</v>
+      </c>
+      <c r="U7" s="32">
+        <v>0</v>
+      </c>
+      <c r="V7" s="30">
+        <v>0</v>
+      </c>
+      <c r="W7" s="31">
+        <v>0</v>
+      </c>
+      <c r="X7" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="34">
-        <v>0</v>
-      </c>
-      <c r="C8" s="35">
-        <v>0</v>
-      </c>
-      <c r="D8" s="35">
-        <v>0</v>
-      </c>
-      <c r="E8" s="35">
-        <v>0</v>
-      </c>
-      <c r="F8" s="36">
-        <v>1</v>
-      </c>
-      <c r="G8" s="34">
-        <v>0</v>
-      </c>
-      <c r="H8" s="35">
-        <v>0</v>
-      </c>
-      <c r="I8" s="35">
-        <v>0</v>
-      </c>
-      <c r="J8" s="35">
-        <v>0</v>
-      </c>
-      <c r="K8" s="36">
-        <v>1</v>
-      </c>
-      <c r="L8" s="34">
-        <v>0</v>
-      </c>
-      <c r="M8" s="35">
-        <v>0</v>
-      </c>
-      <c r="N8" s="35">
-        <v>0</v>
-      </c>
-      <c r="O8" s="35">
-        <v>0</v>
-      </c>
-      <c r="P8" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="34">
-        <v>0</v>
-      </c>
-      <c r="R8" s="35">
-        <v>0</v>
-      </c>
-      <c r="S8" s="35">
-        <v>0</v>
-      </c>
-      <c r="T8" s="35">
-        <v>0</v>
-      </c>
-      <c r="U8" s="36">
-        <v>1</v>
-      </c>
-      <c r="V8" s="34">
-        <v>0</v>
-      </c>
-      <c r="W8" s="35">
-        <v>0</v>
-      </c>
-      <c r="X8" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="36">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="36">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="36">
+      <c r="B8" s="26">
+        <v>0</v>
+      </c>
+      <c r="C8" s="27">
+        <v>0</v>
+      </c>
+      <c r="D8" s="27">
+        <v>0</v>
+      </c>
+      <c r="E8" s="27">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
+        <v>1</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+      <c r="I8" s="27">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0</v>
+      </c>
+      <c r="K8" s="28">
+        <v>1</v>
+      </c>
+      <c r="L8" s="26">
+        <v>0</v>
+      </c>
+      <c r="M8" s="27">
+        <v>0</v>
+      </c>
+      <c r="N8" s="27">
+        <v>0</v>
+      </c>
+      <c r="O8" s="27">
+        <v>0</v>
+      </c>
+      <c r="P8" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>0</v>
+      </c>
+      <c r="R8" s="27">
+        <v>0</v>
+      </c>
+      <c r="S8" s="27">
+        <v>0</v>
+      </c>
+      <c r="T8" s="27">
+        <v>0</v>
+      </c>
+      <c r="U8" s="28">
+        <v>1</v>
+      </c>
+      <c r="V8" s="26">
+        <v>0</v>
+      </c>
+      <c r="W8" s="27">
+        <v>0</v>
+      </c>
+      <c r="X8" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="28">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38">
-        <v>0</v>
-      </c>
-      <c r="C9" s="39">
-        <v>0</v>
-      </c>
-      <c r="D9" s="39">
-        <v>0</v>
-      </c>
-      <c r="E9" s="39">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <v>1</v>
-      </c>
-      <c r="G9" s="38">
-        <v>0</v>
-      </c>
-      <c r="H9" s="39">
-        <v>0</v>
-      </c>
-      <c r="I9" s="39">
-        <v>0</v>
-      </c>
-      <c r="J9" s="39">
-        <v>0</v>
-      </c>
-      <c r="K9" s="40">
-        <v>1</v>
-      </c>
-      <c r="L9" s="38">
-        <v>0</v>
-      </c>
-      <c r="M9" s="39">
-        <v>0</v>
-      </c>
-      <c r="N9" s="39">
-        <v>0</v>
-      </c>
-      <c r="O9" s="39">
-        <v>0</v>
-      </c>
-      <c r="P9" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="38">
-        <v>0</v>
-      </c>
-      <c r="R9" s="39">
-        <v>0</v>
-      </c>
-      <c r="S9" s="39">
-        <v>0</v>
-      </c>
-      <c r="T9" s="39">
-        <v>0</v>
-      </c>
-      <c r="U9" s="40">
-        <v>0</v>
-      </c>
-      <c r="V9" s="38">
-        <v>0</v>
-      </c>
-      <c r="W9" s="39">
-        <v>0</v>
-      </c>
-      <c r="X9" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="40">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="40">
+      <c r="B9" s="30">
+        <v>0</v>
+      </c>
+      <c r="C9" s="31">
+        <v>0</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="30">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31">
+        <v>0</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0</v>
+      </c>
+      <c r="J9" s="31">
+        <v>0</v>
+      </c>
+      <c r="K9" s="32">
+        <v>1</v>
+      </c>
+      <c r="L9" s="30">
+        <v>0</v>
+      </c>
+      <c r="M9" s="31">
+        <v>0</v>
+      </c>
+      <c r="N9" s="31">
+        <v>0</v>
+      </c>
+      <c r="O9" s="31">
+        <v>0</v>
+      </c>
+      <c r="P9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>0</v>
+      </c>
+      <c r="R9" s="31">
+        <v>0</v>
+      </c>
+      <c r="S9" s="31">
+        <v>0</v>
+      </c>
+      <c r="T9" s="31">
+        <v>0</v>
+      </c>
+      <c r="U9" s="32">
+        <v>0</v>
+      </c>
+      <c r="V9" s="30">
+        <v>0</v>
+      </c>
+      <c r="W9" s="31">
+        <v>0</v>
+      </c>
+      <c r="X9" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="32">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="34">
-        <v>0</v>
-      </c>
-      <c r="C10" s="35">
-        <v>0</v>
-      </c>
-      <c r="D10" s="35">
-        <v>1</v>
-      </c>
-      <c r="E10" s="35">
-        <v>0</v>
-      </c>
-      <c r="F10" s="36">
-        <v>1</v>
-      </c>
-      <c r="G10" s="34">
-        <v>0</v>
-      </c>
-      <c r="H10" s="35">
-        <v>0</v>
-      </c>
-      <c r="I10" s="35">
-        <v>1</v>
-      </c>
-      <c r="J10" s="35">
-        <v>0</v>
-      </c>
-      <c r="K10" s="36">
-        <v>1</v>
-      </c>
-      <c r="L10" s="34">
-        <v>0</v>
-      </c>
-      <c r="M10" s="35">
-        <v>0</v>
-      </c>
-      <c r="N10" s="35">
-        <v>1</v>
-      </c>
-      <c r="O10" s="35">
-        <v>0</v>
-      </c>
-      <c r="P10" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="34">
-        <v>0</v>
-      </c>
-      <c r="R10" s="35">
-        <v>0</v>
-      </c>
-      <c r="S10" s="35">
-        <v>1</v>
-      </c>
-      <c r="T10" s="35">
-        <v>0</v>
-      </c>
-      <c r="U10" s="36">
-        <v>1</v>
-      </c>
-      <c r="V10" s="34">
-        <v>0</v>
-      </c>
-      <c r="W10" s="35">
-        <v>0</v>
-      </c>
-      <c r="X10" s="35">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="36">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="36">
+      <c r="B10" s="26">
+        <v>0</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0</v>
+      </c>
+      <c r="D10" s="27">
+        <v>1</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>1</v>
+      </c>
+      <c r="G10" s="26">
+        <v>0</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0</v>
+      </c>
+      <c r="I10" s="27">
+        <v>1</v>
+      </c>
+      <c r="J10" s="27">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28">
+        <v>1</v>
+      </c>
+      <c r="L10" s="26">
+        <v>0</v>
+      </c>
+      <c r="M10" s="27">
+        <v>0</v>
+      </c>
+      <c r="N10" s="27">
+        <v>1</v>
+      </c>
+      <c r="O10" s="27">
+        <v>0</v>
+      </c>
+      <c r="P10" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>0</v>
+      </c>
+      <c r="R10" s="27">
+        <v>0</v>
+      </c>
+      <c r="S10" s="27">
+        <v>1</v>
+      </c>
+      <c r="T10" s="27">
+        <v>0</v>
+      </c>
+      <c r="U10" s="28">
+        <v>1</v>
+      </c>
+      <c r="V10" s="26">
+        <v>0</v>
+      </c>
+      <c r="W10" s="27">
+        <v>0</v>
+      </c>
+      <c r="X10" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="28">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="28">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="38">
-        <v>0</v>
-      </c>
-      <c r="C11" s="39">
-        <v>0</v>
-      </c>
-      <c r="D11" s="39">
-        <v>0</v>
-      </c>
-      <c r="E11" s="39">
-        <v>0</v>
-      </c>
-      <c r="F11" s="40">
-        <v>0</v>
-      </c>
-      <c r="G11" s="38">
-        <v>0</v>
-      </c>
-      <c r="H11" s="39">
-        <v>0</v>
-      </c>
-      <c r="I11" s="39">
-        <v>0</v>
-      </c>
-      <c r="J11" s="39">
-        <v>0</v>
-      </c>
-      <c r="K11" s="40">
-        <v>1</v>
-      </c>
-      <c r="L11" s="38">
-        <v>0</v>
-      </c>
-      <c r="M11" s="39">
-        <v>0</v>
-      </c>
-      <c r="N11" s="39">
-        <v>0</v>
-      </c>
-      <c r="O11" s="39">
-        <v>0</v>
-      </c>
-      <c r="P11" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="38">
-        <v>0</v>
-      </c>
-      <c r="R11" s="39">
-        <v>0</v>
-      </c>
-      <c r="S11" s="39">
-        <v>0</v>
-      </c>
-      <c r="T11" s="39">
-        <v>0</v>
-      </c>
-      <c r="U11" s="40">
-        <v>1</v>
-      </c>
-      <c r="V11" s="38">
-        <v>0</v>
-      </c>
-      <c r="W11" s="39">
-        <v>0</v>
-      </c>
-      <c r="X11" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="40">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="39">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="40">
+      <c r="B11" s="30">
+        <v>0</v>
+      </c>
+      <c r="C11" s="31">
+        <v>0</v>
+      </c>
+      <c r="D11" s="31">
+        <v>0</v>
+      </c>
+      <c r="E11" s="31">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>0</v>
+      </c>
+      <c r="G11" s="30">
+        <v>0</v>
+      </c>
+      <c r="H11" s="31">
+        <v>0</v>
+      </c>
+      <c r="I11" s="31">
+        <v>0</v>
+      </c>
+      <c r="J11" s="31">
+        <v>0</v>
+      </c>
+      <c r="K11" s="32">
+        <v>1</v>
+      </c>
+      <c r="L11" s="30">
+        <v>0</v>
+      </c>
+      <c r="M11" s="31">
+        <v>0</v>
+      </c>
+      <c r="N11" s="31">
+        <v>0</v>
+      </c>
+      <c r="O11" s="31">
+        <v>0</v>
+      </c>
+      <c r="P11" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="30">
+        <v>0</v>
+      </c>
+      <c r="R11" s="31">
+        <v>0</v>
+      </c>
+      <c r="S11" s="31">
+        <v>0</v>
+      </c>
+      <c r="T11" s="31">
+        <v>0</v>
+      </c>
+      <c r="U11" s="32">
+        <v>1</v>
+      </c>
+      <c r="V11" s="30">
+        <v>0</v>
+      </c>
+      <c r="W11" s="31">
+        <v>0</v>
+      </c>
+      <c r="X11" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="32">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="31">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="34">
-        <v>0</v>
-      </c>
-      <c r="C12" s="35">
-        <v>0</v>
-      </c>
-      <c r="D12" s="35">
-        <v>0</v>
-      </c>
-      <c r="E12" s="35">
-        <v>0</v>
-      </c>
-      <c r="F12" s="36">
-        <v>1</v>
-      </c>
-      <c r="G12" s="34">
-        <v>0</v>
-      </c>
-      <c r="H12" s="35">
-        <v>0</v>
-      </c>
-      <c r="I12" s="35">
-        <v>0</v>
-      </c>
-      <c r="J12" s="35">
-        <v>0</v>
-      </c>
-      <c r="K12" s="36">
-        <v>0</v>
-      </c>
-      <c r="L12" s="34">
-        <v>0</v>
-      </c>
-      <c r="M12" s="35">
-        <v>0</v>
-      </c>
-      <c r="N12" s="35">
-        <v>0</v>
-      </c>
-      <c r="O12" s="35">
-        <v>0</v>
-      </c>
-      <c r="P12" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="34">
-        <v>0</v>
-      </c>
-      <c r="R12" s="35">
-        <v>0</v>
-      </c>
-      <c r="S12" s="35">
-        <v>0</v>
-      </c>
-      <c r="T12" s="35">
-        <v>0</v>
-      </c>
-      <c r="U12" s="36">
-        <v>1</v>
-      </c>
-      <c r="V12" s="34">
-        <v>0</v>
-      </c>
-      <c r="W12" s="35">
-        <v>0</v>
-      </c>
-      <c r="X12" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="35">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="36">
-        <v>1</v>
-      </c>
-      <c r="AF12" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="36">
+      <c r="B12" s="26">
+        <v>0</v>
+      </c>
+      <c r="C12" s="27">
+        <v>0</v>
+      </c>
+      <c r="D12" s="27">
+        <v>0</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <v>1</v>
+      </c>
+      <c r="G12" s="26">
+        <v>0</v>
+      </c>
+      <c r="H12" s="27">
+        <v>0</v>
+      </c>
+      <c r="I12" s="27">
+        <v>0</v>
+      </c>
+      <c r="J12" s="27">
+        <v>0</v>
+      </c>
+      <c r="K12" s="28">
+        <v>0</v>
+      </c>
+      <c r="L12" s="26">
+        <v>0</v>
+      </c>
+      <c r="M12" s="27">
+        <v>0</v>
+      </c>
+      <c r="N12" s="27">
+        <v>0</v>
+      </c>
+      <c r="O12" s="27">
+        <v>0</v>
+      </c>
+      <c r="P12" s="28">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="26">
+        <v>0</v>
+      </c>
+      <c r="R12" s="27">
+        <v>0</v>
+      </c>
+      <c r="S12" s="27">
+        <v>0</v>
+      </c>
+      <c r="T12" s="27">
+        <v>0</v>
+      </c>
+      <c r="U12" s="28">
+        <v>1</v>
+      </c>
+      <c r="V12" s="26">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27">
+        <v>0</v>
+      </c>
+      <c r="X12" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="28">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="28">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="38">
-        <v>0</v>
-      </c>
-      <c r="C13" s="39">
-        <v>1</v>
-      </c>
-      <c r="D13" s="39">
-        <v>0</v>
-      </c>
-      <c r="E13" s="39">
-        <v>0</v>
-      </c>
-      <c r="F13" s="40">
-        <v>0</v>
-      </c>
-      <c r="G13" s="38">
-        <v>0</v>
-      </c>
-      <c r="H13" s="39">
-        <v>1</v>
-      </c>
-      <c r="I13" s="39">
-        <v>0</v>
-      </c>
-      <c r="J13" s="39">
-        <v>0</v>
-      </c>
-      <c r="K13" s="40">
-        <v>0</v>
-      </c>
-      <c r="L13" s="38">
-        <v>0</v>
-      </c>
-      <c r="M13" s="39">
-        <v>0</v>
-      </c>
-      <c r="N13" s="39">
-        <v>0</v>
-      </c>
-      <c r="O13" s="39">
-        <v>0</v>
-      </c>
-      <c r="P13" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="38">
-        <v>0</v>
-      </c>
-      <c r="R13" s="39">
-        <v>1</v>
-      </c>
-      <c r="S13" s="39">
-        <v>0</v>
-      </c>
-      <c r="T13" s="39">
-        <v>0</v>
-      </c>
-      <c r="U13" s="40">
-        <v>0</v>
-      </c>
-      <c r="V13" s="38">
-        <v>0</v>
-      </c>
-      <c r="W13" s="39">
-        <v>0</v>
-      </c>
-      <c r="X13" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="39">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="39">
-        <v>1</v>
-      </c>
-      <c r="AH13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="40">
+      <c r="B13" s="30">
+        <v>0</v>
+      </c>
+      <c r="C13" s="31">
+        <v>1</v>
+      </c>
+      <c r="D13" s="31">
+        <v>0</v>
+      </c>
+      <c r="E13" s="31">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32">
+        <v>0</v>
+      </c>
+      <c r="G13" s="30">
+        <v>0</v>
+      </c>
+      <c r="H13" s="31">
+        <v>1</v>
+      </c>
+      <c r="I13" s="31">
+        <v>0</v>
+      </c>
+      <c r="J13" s="31">
+        <v>0</v>
+      </c>
+      <c r="K13" s="32">
+        <v>0</v>
+      </c>
+      <c r="L13" s="30">
+        <v>0</v>
+      </c>
+      <c r="M13" s="31">
+        <v>0</v>
+      </c>
+      <c r="N13" s="31">
+        <v>0</v>
+      </c>
+      <c r="O13" s="31">
+        <v>0</v>
+      </c>
+      <c r="P13" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="30">
+        <v>0</v>
+      </c>
+      <c r="R13" s="31">
+        <v>1</v>
+      </c>
+      <c r="S13" s="31">
+        <v>0</v>
+      </c>
+      <c r="T13" s="31">
+        <v>0</v>
+      </c>
+      <c r="U13" s="32">
+        <v>0</v>
+      </c>
+      <c r="V13" s="30">
+        <v>0</v>
+      </c>
+      <c r="W13" s="31">
+        <v>0</v>
+      </c>
+      <c r="X13" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="31">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="34">
-        <v>0</v>
-      </c>
-      <c r="C14" s="35">
-        <v>0</v>
-      </c>
-      <c r="D14" s="35">
-        <v>0</v>
-      </c>
-      <c r="E14" s="35">
-        <v>0</v>
-      </c>
-      <c r="F14" s="36">
-        <v>0</v>
-      </c>
-      <c r="G14" s="34">
-        <v>0</v>
-      </c>
-      <c r="H14" s="35">
-        <v>0</v>
-      </c>
-      <c r="I14" s="35">
-        <v>0</v>
-      </c>
-      <c r="J14" s="35">
-        <v>0</v>
-      </c>
-      <c r="K14" s="36">
-        <v>0</v>
-      </c>
-      <c r="L14" s="34">
-        <v>0</v>
-      </c>
-      <c r="M14" s="35">
-        <v>0</v>
-      </c>
-      <c r="N14" s="35">
-        <v>0</v>
-      </c>
-      <c r="O14" s="35">
-        <v>0</v>
-      </c>
-      <c r="P14" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="34">
-        <v>0</v>
-      </c>
-      <c r="R14" s="35">
-        <v>0</v>
-      </c>
-      <c r="S14" s="35">
-        <v>0</v>
-      </c>
-      <c r="T14" s="35">
-        <v>0</v>
-      </c>
-      <c r="U14" s="36">
-        <v>0</v>
-      </c>
-      <c r="V14" s="34">
-        <v>0</v>
-      </c>
-      <c r="W14" s="35">
-        <v>0</v>
-      </c>
-      <c r="X14" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="36">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="36">
+      <c r="B14" s="26">
+        <v>0</v>
+      </c>
+      <c r="C14" s="27">
+        <v>0</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0</v>
+      </c>
+      <c r="G14" s="26">
+        <v>0</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0</v>
+      </c>
+      <c r="J14" s="27">
+        <v>0</v>
+      </c>
+      <c r="K14" s="28">
+        <v>0</v>
+      </c>
+      <c r="L14" s="26">
+        <v>0</v>
+      </c>
+      <c r="M14" s="27">
+        <v>0</v>
+      </c>
+      <c r="N14" s="27">
+        <v>0</v>
+      </c>
+      <c r="O14" s="27">
+        <v>0</v>
+      </c>
+      <c r="P14" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>0</v>
+      </c>
+      <c r="R14" s="27">
+        <v>0</v>
+      </c>
+      <c r="S14" s="27">
+        <v>0</v>
+      </c>
+      <c r="T14" s="27">
+        <v>0</v>
+      </c>
+      <c r="U14" s="28">
+        <v>0</v>
+      </c>
+      <c r="V14" s="26">
+        <v>0</v>
+      </c>
+      <c r="W14" s="27">
+        <v>0</v>
+      </c>
+      <c r="X14" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="28">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="28">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="38">
-        <v>0</v>
-      </c>
-      <c r="C15" s="39">
-        <v>0</v>
-      </c>
-      <c r="D15" s="39">
-        <v>1</v>
-      </c>
-      <c r="E15" s="39">
-        <v>0</v>
-      </c>
-      <c r="F15" s="40">
-        <v>0</v>
-      </c>
-      <c r="G15" s="38">
-        <v>0</v>
-      </c>
-      <c r="H15" s="39">
-        <v>0</v>
-      </c>
-      <c r="I15" s="39">
-        <v>0</v>
-      </c>
-      <c r="J15" s="39">
-        <v>0</v>
-      </c>
-      <c r="K15" s="40">
-        <v>1</v>
-      </c>
-      <c r="L15" s="38">
-        <v>0</v>
-      </c>
-      <c r="M15" s="39">
-        <v>0</v>
-      </c>
-      <c r="N15" s="39">
-        <v>0</v>
-      </c>
-      <c r="O15" s="39">
-        <v>0</v>
-      </c>
-      <c r="P15" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="38">
-        <v>0</v>
-      </c>
-      <c r="R15" s="39">
-        <v>0</v>
-      </c>
-      <c r="S15" s="39">
-        <v>1</v>
-      </c>
-      <c r="T15" s="39">
-        <v>0</v>
-      </c>
-      <c r="U15" s="40">
-        <v>0</v>
-      </c>
-      <c r="V15" s="38">
-        <v>0</v>
-      </c>
-      <c r="W15" s="39">
-        <v>0</v>
-      </c>
-      <c r="X15" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="39">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="40">
+      <c r="B15" s="30">
+        <v>0</v>
+      </c>
+      <c r="C15" s="31">
+        <v>0</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30">
+        <v>0</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0</v>
+      </c>
+      <c r="J15" s="31">
+        <v>0</v>
+      </c>
+      <c r="K15" s="32">
+        <v>1</v>
+      </c>
+      <c r="L15" s="30">
+        <v>0</v>
+      </c>
+      <c r="M15" s="31">
+        <v>0</v>
+      </c>
+      <c r="N15" s="31">
+        <v>0</v>
+      </c>
+      <c r="O15" s="31">
+        <v>0</v>
+      </c>
+      <c r="P15" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>0</v>
+      </c>
+      <c r="R15" s="31">
+        <v>0</v>
+      </c>
+      <c r="S15" s="31">
+        <v>1</v>
+      </c>
+      <c r="T15" s="31">
+        <v>0</v>
+      </c>
+      <c r="U15" s="32">
+        <v>0</v>
+      </c>
+      <c r="V15" s="30">
+        <v>0</v>
+      </c>
+      <c r="W15" s="31">
+        <v>0</v>
+      </c>
+      <c r="X15" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="31">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="34">
-        <v>0</v>
-      </c>
-      <c r="C16" s="35">
-        <v>0</v>
-      </c>
-      <c r="D16" s="35">
-        <v>0</v>
-      </c>
-      <c r="E16" s="35">
-        <v>0</v>
-      </c>
-      <c r="F16" s="36">
-        <v>0</v>
-      </c>
-      <c r="G16" s="34">
-        <v>0</v>
-      </c>
-      <c r="H16" s="35">
-        <v>0</v>
-      </c>
-      <c r="I16" s="35">
-        <v>0</v>
-      </c>
-      <c r="J16" s="35">
-        <v>0</v>
-      </c>
-      <c r="K16" s="36">
-        <v>0</v>
-      </c>
-      <c r="L16" s="34">
-        <v>0</v>
-      </c>
-      <c r="M16" s="35">
-        <v>0</v>
-      </c>
-      <c r="N16" s="35">
-        <v>0</v>
-      </c>
-      <c r="O16" s="35">
-        <v>0</v>
-      </c>
-      <c r="P16" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="34">
-        <v>0</v>
-      </c>
-      <c r="R16" s="35">
-        <v>0</v>
-      </c>
-      <c r="S16" s="35">
-        <v>0</v>
-      </c>
-      <c r="T16" s="35">
-        <v>0</v>
-      </c>
-      <c r="U16" s="36">
-        <v>0</v>
-      </c>
-      <c r="V16" s="34">
-        <v>0</v>
-      </c>
-      <c r="W16" s="35">
-        <v>0</v>
-      </c>
-      <c r="X16" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="36">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="36">
+      <c r="B16" s="26">
+        <v>0</v>
+      </c>
+      <c r="C16" s="27">
+        <v>0</v>
+      </c>
+      <c r="D16" s="27">
+        <v>0</v>
+      </c>
+      <c r="E16" s="27">
+        <v>0</v>
+      </c>
+      <c r="F16" s="28">
+        <v>0</v>
+      </c>
+      <c r="G16" s="26">
+        <v>0</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0</v>
+      </c>
+      <c r="I16" s="27">
+        <v>0</v>
+      </c>
+      <c r="J16" s="27">
+        <v>0</v>
+      </c>
+      <c r="K16" s="28">
+        <v>0</v>
+      </c>
+      <c r="L16" s="26">
+        <v>0</v>
+      </c>
+      <c r="M16" s="27">
+        <v>0</v>
+      </c>
+      <c r="N16" s="27">
+        <v>0</v>
+      </c>
+      <c r="O16" s="27">
+        <v>0</v>
+      </c>
+      <c r="P16" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="26">
+        <v>0</v>
+      </c>
+      <c r="R16" s="27">
+        <v>0</v>
+      </c>
+      <c r="S16" s="27">
+        <v>0</v>
+      </c>
+      <c r="T16" s="27">
+        <v>0</v>
+      </c>
+      <c r="U16" s="28">
+        <v>0</v>
+      </c>
+      <c r="V16" s="26">
+        <v>0</v>
+      </c>
+      <c r="W16" s="27">
+        <v>0</v>
+      </c>
+      <c r="X16" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="28">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="28">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="38">
-        <v>0</v>
-      </c>
-      <c r="C17" s="39">
-        <v>1</v>
-      </c>
-      <c r="D17" s="39">
-        <v>0</v>
-      </c>
-      <c r="E17" s="39">
-        <v>0</v>
-      </c>
-      <c r="F17" s="40">
-        <v>1</v>
-      </c>
-      <c r="G17" s="38">
-        <v>0</v>
-      </c>
-      <c r="H17" s="39">
-        <v>1</v>
-      </c>
-      <c r="I17" s="39">
-        <v>0</v>
-      </c>
-      <c r="J17" s="39">
-        <v>0</v>
-      </c>
-      <c r="K17" s="40">
-        <v>1</v>
-      </c>
-      <c r="L17" s="38">
-        <v>0</v>
-      </c>
-      <c r="M17" s="39">
-        <v>1</v>
-      </c>
-      <c r="N17" s="39">
-        <v>0</v>
-      </c>
-      <c r="O17" s="39">
-        <v>0</v>
-      </c>
-      <c r="P17" s="40">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="38">
-        <v>0</v>
-      </c>
-      <c r="R17" s="39">
-        <v>1</v>
-      </c>
-      <c r="S17" s="39">
-        <v>0</v>
-      </c>
-      <c r="T17" s="39">
-        <v>0</v>
-      </c>
-      <c r="U17" s="40">
-        <v>1</v>
-      </c>
-      <c r="V17" s="38">
-        <v>0</v>
-      </c>
-      <c r="W17" s="39">
-        <v>1</v>
-      </c>
-      <c r="X17" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="39">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="38">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="40">
+      <c r="B17" s="30">
+        <v>0</v>
+      </c>
+      <c r="C17" s="31">
+        <v>1</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0</v>
+      </c>
+      <c r="E17" s="31">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>1</v>
+      </c>
+      <c r="G17" s="30">
+        <v>0</v>
+      </c>
+      <c r="H17" s="31">
+        <v>1</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0</v>
+      </c>
+      <c r="J17" s="31">
+        <v>0</v>
+      </c>
+      <c r="K17" s="32">
+        <v>1</v>
+      </c>
+      <c r="L17" s="30">
+        <v>0</v>
+      </c>
+      <c r="M17" s="31">
+        <v>1</v>
+      </c>
+      <c r="N17" s="31">
+        <v>0</v>
+      </c>
+      <c r="O17" s="31">
+        <v>0</v>
+      </c>
+      <c r="P17" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>0</v>
+      </c>
+      <c r="R17" s="31">
+        <v>1</v>
+      </c>
+      <c r="S17" s="31">
+        <v>0</v>
+      </c>
+      <c r="T17" s="31">
+        <v>0</v>
+      </c>
+      <c r="U17" s="32">
+        <v>1</v>
+      </c>
+      <c r="V17" s="30">
+        <v>0</v>
+      </c>
+      <c r="W17" s="31">
+        <v>1</v>
+      </c>
+      <c r="X17" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="31">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="34">
-        <v>0</v>
-      </c>
-      <c r="C18" s="35">
-        <v>1</v>
-      </c>
-      <c r="D18" s="35">
-        <v>0</v>
-      </c>
-      <c r="E18" s="35">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36">
-        <v>0</v>
-      </c>
-      <c r="G18" s="34">
-        <v>0</v>
-      </c>
-      <c r="H18" s="35">
-        <v>1</v>
-      </c>
-      <c r="I18" s="35">
-        <v>0</v>
-      </c>
-      <c r="J18" s="35">
-        <v>0</v>
-      </c>
-      <c r="K18" s="36">
-        <v>0</v>
-      </c>
-      <c r="L18" s="34">
-        <v>0</v>
-      </c>
-      <c r="M18" s="35">
-        <v>1</v>
-      </c>
-      <c r="N18" s="35">
-        <v>0</v>
-      </c>
-      <c r="O18" s="35">
-        <v>0</v>
-      </c>
-      <c r="P18" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="34">
-        <v>0</v>
-      </c>
-      <c r="R18" s="35">
-        <v>1</v>
-      </c>
-      <c r="S18" s="35">
-        <v>0</v>
-      </c>
-      <c r="T18" s="35">
-        <v>0</v>
-      </c>
-      <c r="U18" s="36">
-        <v>0</v>
-      </c>
-      <c r="V18" s="34">
-        <v>0</v>
-      </c>
-      <c r="W18" s="35">
-        <v>1</v>
-      </c>
-      <c r="X18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="36">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="36">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="34">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="36">
+      <c r="B18" s="26">
+        <v>0</v>
+      </c>
+      <c r="C18" s="27">
+        <v>1</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0</v>
+      </c>
+      <c r="E18" s="27">
+        <v>0</v>
+      </c>
+      <c r="F18" s="28">
+        <v>0</v>
+      </c>
+      <c r="G18" s="26">
+        <v>0</v>
+      </c>
+      <c r="H18" s="27">
+        <v>1</v>
+      </c>
+      <c r="I18" s="27">
+        <v>0</v>
+      </c>
+      <c r="J18" s="27">
+        <v>0</v>
+      </c>
+      <c r="K18" s="28">
+        <v>0</v>
+      </c>
+      <c r="L18" s="26">
+        <v>0</v>
+      </c>
+      <c r="M18" s="27">
+        <v>1</v>
+      </c>
+      <c r="N18" s="27">
+        <v>0</v>
+      </c>
+      <c r="O18" s="27">
+        <v>0</v>
+      </c>
+      <c r="P18" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>0</v>
+      </c>
+      <c r="R18" s="27">
+        <v>1</v>
+      </c>
+      <c r="S18" s="27">
+        <v>0</v>
+      </c>
+      <c r="T18" s="27">
+        <v>0</v>
+      </c>
+      <c r="U18" s="28">
+        <v>0</v>
+      </c>
+      <c r="V18" s="26">
+        <v>0</v>
+      </c>
+      <c r="W18" s="27">
+        <v>1</v>
+      </c>
+      <c r="X18" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="28">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="28">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="42">
-        <v>0</v>
-      </c>
-      <c r="C19" s="43">
-        <v>0</v>
-      </c>
-      <c r="D19" s="43">
-        <v>1</v>
-      </c>
-      <c r="E19" s="43">
-        <v>0</v>
-      </c>
-      <c r="F19" s="44">
-        <v>0</v>
-      </c>
-      <c r="G19" s="42">
-        <v>0</v>
-      </c>
-      <c r="H19" s="43">
-        <v>0</v>
-      </c>
-      <c r="I19" s="43">
-        <v>1</v>
-      </c>
-      <c r="J19" s="43">
-        <v>0</v>
-      </c>
-      <c r="K19" s="44">
-        <v>0</v>
-      </c>
-      <c r="L19" s="42">
-        <v>0</v>
-      </c>
-      <c r="M19" s="43">
-        <v>0</v>
-      </c>
-      <c r="N19" s="43">
-        <v>0</v>
-      </c>
-      <c r="O19" s="43">
-        <v>0</v>
-      </c>
-      <c r="P19" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="42">
-        <v>0</v>
-      </c>
-      <c r="R19" s="43">
-        <v>0</v>
-      </c>
-      <c r="S19" s="43">
-        <v>1</v>
-      </c>
-      <c r="T19" s="43">
-        <v>0</v>
-      </c>
-      <c r="U19" s="44">
-        <v>0</v>
-      </c>
-      <c r="V19" s="42">
-        <v>0</v>
-      </c>
-      <c r="W19" s="43">
-        <v>0</v>
-      </c>
-      <c r="X19" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="43">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="44">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="42">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="43">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="43">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="43">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF19" s="42">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="43">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="43">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="43">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="44">
+      <c r="B19" s="34">
+        <v>0</v>
+      </c>
+      <c r="C19" s="35">
+        <v>0</v>
+      </c>
+      <c r="D19" s="35">
+        <v>1</v>
+      </c>
+      <c r="E19" s="35">
+        <v>0</v>
+      </c>
+      <c r="F19" s="36">
+        <v>0</v>
+      </c>
+      <c r="G19" s="34">
+        <v>0</v>
+      </c>
+      <c r="H19" s="35">
+        <v>0</v>
+      </c>
+      <c r="I19" s="35">
+        <v>1</v>
+      </c>
+      <c r="J19" s="35">
+        <v>0</v>
+      </c>
+      <c r="K19" s="36">
+        <v>0</v>
+      </c>
+      <c r="L19" s="34">
+        <v>0</v>
+      </c>
+      <c r="M19" s="35">
+        <v>0</v>
+      </c>
+      <c r="N19" s="35">
+        <v>0</v>
+      </c>
+      <c r="O19" s="35">
+        <v>0</v>
+      </c>
+      <c r="P19" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="34">
+        <v>0</v>
+      </c>
+      <c r="R19" s="35">
+        <v>0</v>
+      </c>
+      <c r="S19" s="35">
+        <v>1</v>
+      </c>
+      <c r="T19" s="35">
+        <v>0</v>
+      </c>
+      <c r="U19" s="36">
+        <v>0</v>
+      </c>
+      <c r="V19" s="34">
+        <v>0</v>
+      </c>
+      <c r="W19" s="35">
+        <v>0</v>
+      </c>
+      <c r="X19" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="35">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="36">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="34">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="35">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="35">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="36">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3563,54 +3563,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="21" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="21" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="21" t="s">
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="21" t="s">
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="21" t="s">
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="21" t="s">
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="23"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="55"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" s="25"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Finished electricity profile and creating domestic hot water profile.
</commit_message>
<xml_diff>
--- a/Electricity.xlsx
+++ b/Electricity.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF0E5D-3231-49E9-9C65-CA14C400ECDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5B712-ADB2-4459-A92C-95F73E0748BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Summer" sheetId="2" r:id="rId2"/>
-    <sheet name="Winter" sheetId="4" r:id="rId3"/>
+    <sheet name="Heat Pump" sheetId="5" r:id="rId2"/>
+    <sheet name="Summer" sheetId="2" r:id="rId3"/>
+    <sheet name="Winter" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="autoNoTable"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="46">
   <si>
     <t>Appliance</t>
   </si>
@@ -170,6 +171,12 @@
   </si>
   <si>
     <t>Night 2</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>COP</t>
   </si>
 </sst>
 </file>
@@ -966,7 +973,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,7 +1080,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -1113,7 +1120,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -1133,7 +1140,7 @@
         <v>90</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -1153,7 +1160,7 @@
         <v>90</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -1173,7 +1180,7 @@
         <v>120</v>
       </c>
       <c r="E10" s="3">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -1194,7 +1201,7 @@
         <v>240</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -1214,7 +1221,7 @@
         <v>60</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -1234,7 +1241,7 @@
         <v>60</v>
       </c>
       <c r="E13" s="3">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3">
         <v>0</v>
@@ -1254,7 +1261,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="F14" s="3">
         <v>0</v>
@@ -1274,7 +1281,7 @@
         <v>120</v>
       </c>
       <c r="E15" s="3">
-        <v>1</v>
+        <v>320</v>
       </c>
       <c r="F15" s="3">
         <v>12</v>
@@ -1294,7 +1301,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="3">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F16" s="3">
         <v>3</v>
@@ -1315,7 +1322,7 @@
         <v>240</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="F17" s="3">
         <v>3</v>
@@ -1336,7 +1343,7 @@
         <v>180</v>
       </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
@@ -1356,7 +1363,7 @@
         <v>120</v>
       </c>
       <c r="E19" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
@@ -1376,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="3">
-        <v>1</v>
+        <v>360</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
@@ -1396,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F21" s="3">
         <v>0</v>
@@ -1416,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="3">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="F22" s="3">
         <v>4</v>
@@ -1432,14 +1439,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84531F1-D93A-4AD3-91D2-2A0C2792D38A}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>-15</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>-10</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>-5</v>
+      </c>
+      <c r="B4">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>4.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EEF8B1-E0DF-4071-B506-FDD79B5129C3}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1793,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="39">
         <v>1</v>
@@ -1903,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="31">
         <v>0</v>
@@ -1968,7 +2073,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -2013,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="27">
         <v>0</v>
@@ -2123,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="31">
         <v>0</v>
@@ -2233,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="27">
         <v>0</v>
@@ -2343,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="31">
         <v>0</v>
@@ -2453,7 +2558,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="27">
         <v>0</v>
@@ -2563,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="31">
         <v>0</v>
@@ -2673,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="Q12" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="27">
         <v>0</v>
@@ -2783,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="31">
         <v>1</v>
@@ -2893,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="27">
         <v>0</v>
@@ -3003,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="31">
         <v>0</v>
@@ -3113,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="27">
         <v>0</v>
@@ -3223,7 +3328,7 @@
         <v>1</v>
       </c>
       <c r="Q17" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="31">
         <v>1</v>
@@ -3333,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="27">
         <v>1</v>
@@ -3443,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="35">
         <v>0</v>
@@ -3518,7 +3623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BDE5F3-3401-4093-8A81-1C2CE3A9CE8F}">
   <dimension ref="A1:AC19"/>
   <sheetViews>

</xml_diff>

<commit_message>
DHW, Optimisation and Orientation Changes
Updated DHW consumption profile methodology and started writing optimisation.
</commit_message>
<xml_diff>
--- a/Electricity.xlsx
+++ b/Electricity.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5B712-ADB2-4459-A92C-95F73E0748BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2614A833-4333-44EA-857C-9049C6B457F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Heat Pump" sheetId="5" r:id="rId2"/>
-    <sheet name="Summer" sheetId="2" r:id="rId3"/>
-    <sheet name="Winter" sheetId="4" r:id="rId4"/>
+    <sheet name="Costs" sheetId="6" r:id="rId3"/>
+    <sheet name="Summer" sheetId="2" r:id="rId4"/>
+    <sheet name="Winter" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" calcMode="autoNoTable"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="51">
   <si>
     <t>Appliance</t>
   </si>
@@ -178,6 +180,21 @@
   <si>
     <t>COP</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>CCL (£/kWh)</t>
+  </si>
+  <si>
+    <t>Export Income (£/kWh)</t>
+  </si>
+  <si>
+    <t>Import Cost (£/kWh)</t>
+  </si>
 </sst>
 </file>
 
@@ -515,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -615,6 +632,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -962,7 +982,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1442,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84531F1-D93A-4AD3-91D2-2A0C2792D38A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1537,6 +1557,57 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228E9AC0-CE01-4C51-9B82-0E67C0BBA7C6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EEF8B1-E0DF-4071-B506-FDD79B5129C3}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
@@ -1577,61 +1648,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="50" t="s">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="45" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="45" t="s">
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="45" t="s">
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="45" t="s">
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="45" t="s">
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="45" t="s">
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="48"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A2" s="49"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="22" t="s">
         <v>42</v>
       </c>
@@ -3623,7 +3694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BDE5F3-3401-4093-8A81-1C2CE3A9CE8F}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3668,54 +3739,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53" t="s">
+      <c r="A1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="53" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="53" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="53" t="s">
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="53" t="s">
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="53" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="53" t="s">
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="56"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" s="57"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Included 20 year generation analysis for IRR and NPV.
</commit_message>
<xml_diff>
--- a/Electricity.xlsx
+++ b/Electricity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2614A833-4333-44EA-857C-9049C6B457F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A451718A-1920-4DF3-89E2-FEF6CE88B9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Winter" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" calcMode="autoNoTable"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1462,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84531F1-D93A-4AD3-91D2-2A0C2792D38A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1560,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228E9AC0-CE01-4C51-9B82-0E67C0BBA7C6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added thermal storage leakage and added heat pump cooling with constant COP
</commit_message>
<xml_diff>
--- a/Electricity.xlsx
+++ b/Electricity.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A451718A-1920-4DF3-89E2-FEF6CE88B9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BAC1F7-D4B2-4332-951A-A9C4819DAF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{9D626799-2A6E-48CA-90B6-E677FE61AA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Heat Pump" sheetId="5" r:id="rId2"/>
-    <sheet name="Costs" sheetId="6" r:id="rId3"/>
-    <sheet name="Summer" sheetId="2" r:id="rId4"/>
-    <sheet name="Winter" sheetId="4" r:id="rId5"/>
+    <sheet name="Summer" sheetId="2" r:id="rId3"/>
+    <sheet name="Winter" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" calcMode="autoNoTable"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="46">
   <si>
     <t>Appliance</t>
   </si>
@@ -179,21 +178,6 @@
   <si>
     <t>COP</t>
   </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>CCL (£/kWh)</t>
-  </si>
-  <si>
-    <t>Export Income (£/kWh)</t>
-  </si>
-  <si>
-    <t>Import Cost (£/kWh)</t>
-  </si>
 </sst>
 </file>
 
@@ -531,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -631,9 +615,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1461,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84531F1-D93A-4AD3-91D2-2A0C2792D38A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1556,61 +1537,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228E9AC0-CE01-4C51-9B82-0E67C0BBA7C6}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
-        <v>7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
-        <v>0.05</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EEF8B1-E0DF-4071-B506-FDD79B5129C3}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1647,61 +1577,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51" t="s">
+      <c r="A1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="46" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="46" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="46" t="s">
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="46" t="s">
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="46" t="s">
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="46" t="s">
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="47"/>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="48"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="47"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A2" s="50"/>
+      <c r="A2" s="49"/>
       <c r="B2" s="22" t="s">
         <v>42</v>
       </c>
@@ -3693,7 +3623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BDE5F3-3401-4093-8A81-1C2CE3A9CE8F}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
@@ -3738,54 +3668,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="54" t="s">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="54" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="54" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="54" t="s">
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="54" t="s">
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="54" t="s">
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="54" t="s">
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="56"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="55"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" s="58"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>